<commit_message>
add sh: default namespace for xlsx2shape. close #15
</commit_message>
<xml_diff>
--- a/spec/example/example.xlsx
+++ b/spec/example/example.xlsx
@@ -12,8 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10536"/>
   </bookViews>
   <sheets>
-    <sheet name="Prefix" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>https://example.org/Ashape</t>
     <phoneticPr fontId="1"/>
@@ -48,14 +47,6 @@
   </si>
   <si>
     <t>sh:targetClass</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>sh:</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>http://www.w3.org/ns/shacl#</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -402,36 +393,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>